<commit_message>
sort the orderline by line number
</commit_message>
<xml_diff>
--- a/results/PO/PO_HIT.xlsx
+++ b/results/PO/PO_HIT.xlsx
@@ -180,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -581,6 +581,20 @@
         <color indexed="64"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -602,6 +616,30 @@
       <top style="thin">
         <color rgb="00000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="medium"/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
       <bottom style="medium"/>
     </border>
     <border>
@@ -618,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -990,7 +1028,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1000,7 +1038,20 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1461,7 +1512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" workbookViewId="0">
       <selection activeCell="R19" sqref="R19"/>
@@ -1547,7 +1598,7 @@
       </c>
       <c r="R2" s="132" t="inlineStr">
         <is>
-          <t>po</t>
+          <t>aaaa</t>
         </is>
       </c>
     </row>
@@ -1796,11 +1847,7 @@
       <c r="M12" s="52" t="n"/>
       <c r="N12" s="52" t="n"/>
       <c r="O12" s="53" t="n"/>
-      <c r="P12" s="140" t="inlineStr">
-        <is>
-          <t>addline4</t>
-        </is>
-      </c>
+      <c r="P12" s="140" t="inlineStr"/>
       <c r="Q12" s="52" t="n"/>
       <c r="R12" s="52" t="n"/>
       <c r="S12" s="141" t="n"/>
@@ -2067,226 +2114,426 @@
         </is>
       </c>
       <c r="C17" s="150" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D17" s="151" t="n"/>
       <c r="E17" s="150" t="inlineStr">
         <is>
-          <t>PN</t>
+          <t>22002</t>
         </is>
       </c>
       <c r="F17" s="150" t="inlineStr"/>
       <c r="G17" s="150" t="inlineStr"/>
       <c r="H17" s="151" t="n"/>
       <c r="I17" s="151" t="n"/>
-      <c r="J17" s="150" t="inlineStr"/>
-      <c r="K17" s="150" t="inlineStr"/>
+      <c r="J17" s="150" t="inlineStr">
+        <is>
+          <t>INSERT</t>
+        </is>
+      </c>
+      <c r="K17" s="150" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
       <c r="L17" s="150" t="inlineStr">
         <is>
           <t>Sea</t>
         </is>
       </c>
       <c r="M17" s="152" t="n">
-        <v>45561</v>
+        <v>45554</v>
       </c>
       <c r="N17" s="150" t="n"/>
       <c r="O17" s="150" t="n"/>
       <c r="P17" s="151" t="n"/>
       <c r="Q17" s="150" t="n">
-        <v>200</v>
+        <v>13.26</v>
       </c>
       <c r="R17" s="151" t="n"/>
       <c r="S17" s="153" t="n">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="18" ht="6" customHeight="1">
-      <c r="B18" s="13" t="n"/>
-      <c r="C18" s="14" t="n"/>
-      <c r="D18" s="9" t="n"/>
-      <c r="E18" s="15" t="n"/>
-      <c r="F18" s="15" t="n"/>
-      <c r="G18" s="8" t="n"/>
-      <c r="H18" s="8" t="n"/>
-      <c r="I18" s="8" t="n"/>
-      <c r="J18" s="10" t="n"/>
-      <c r="K18" s="101" t="n"/>
-      <c r="L18" s="9" t="n"/>
-      <c r="M18" s="154" t="n"/>
-      <c r="N18" s="154" t="n"/>
-      <c r="O18" s="31" t="n"/>
-      <c r="P18" s="155" t="n"/>
-      <c r="Q18" s="155" t="n"/>
-      <c r="R18" s="155" t="n"/>
-      <c r="S18" s="156" t="n"/>
-    </row>
-    <row r="19" ht="16" customHeight="1" thickBot="1">
-      <c r="B19" s="13" t="n"/>
-      <c r="C19" s="14" t="n"/>
-      <c r="D19" s="9" t="n"/>
-      <c r="E19" s="15" t="n"/>
-      <c r="F19" s="15" t="n"/>
-      <c r="G19" s="8" t="n"/>
-      <c r="H19" s="8" t="n"/>
-      <c r="I19" s="8" t="n"/>
-      <c r="J19" s="10" t="n"/>
-      <c r="K19" s="101" t="n"/>
-      <c r="L19" s="9" t="n"/>
-      <c r="M19" s="154" t="n"/>
-      <c r="N19" s="154" t="n"/>
-      <c r="O19" s="31" t="n"/>
-      <c r="P19" s="155" t="n"/>
-      <c r="Q19" s="155" t="n"/>
-      <c r="R19" s="155" t="n"/>
-      <c r="S19" s="156" t="n"/>
-    </row>
-    <row r="20" ht="16" customHeight="1" thickTop="1">
-      <c r="M20" s="17" t="n"/>
-      <c r="N20" s="33" t="n"/>
-      <c r="O20" s="33" t="n"/>
-      <c r="P20" s="79" t="inlineStr">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1">
+      <c r="B18" s="149" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C18" s="150" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D18" s="151" t="n"/>
+      <c r="E18" s="150" t="inlineStr">
+        <is>
+          <t>22002</t>
+        </is>
+      </c>
+      <c r="F18" s="150" t="inlineStr"/>
+      <c r="G18" s="150" t="inlineStr"/>
+      <c r="H18" s="151" t="n"/>
+      <c r="I18" s="151" t="n"/>
+      <c r="J18" s="150" t="inlineStr">
+        <is>
+          <t>INSERT</t>
+        </is>
+      </c>
+      <c r="K18" s="150" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="L18" s="150" t="inlineStr">
+        <is>
+          <t>Sea</t>
+        </is>
+      </c>
+      <c r="M18" s="152" t="n">
+        <v>45554</v>
+      </c>
+      <c r="N18" s="150" t="n"/>
+      <c r="O18" s="150" t="n"/>
+      <c r="P18" s="151" t="n"/>
+      <c r="Q18" s="150" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="R18" s="151" t="n"/>
+      <c r="S18" s="153" t="n">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1" thickBot="1">
+      <c r="B19" s="149" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C19" s="150" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D19" s="151" t="n"/>
+      <c r="E19" s="150" t="inlineStr">
+        <is>
+          <t>22002</t>
+        </is>
+      </c>
+      <c r="F19" s="150" t="inlineStr"/>
+      <c r="G19" s="150" t="inlineStr"/>
+      <c r="H19" s="151" t="n"/>
+      <c r="I19" s="151" t="n"/>
+      <c r="J19" s="150" t="inlineStr">
+        <is>
+          <t>INSERT</t>
+        </is>
+      </c>
+      <c r="K19" s="150" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="L19" s="150" t="inlineStr">
+        <is>
+          <t>Sea</t>
+        </is>
+      </c>
+      <c r="M19" s="152" t="n">
+        <v>45554</v>
+      </c>
+      <c r="N19" s="150" t="n"/>
+      <c r="O19" s="150" t="n"/>
+      <c r="P19" s="151" t="n"/>
+      <c r="Q19" s="150" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="R19" s="151" t="n"/>
+      <c r="S19" s="153" t="n">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1" thickTop="1">
+      <c r="B20" s="149" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C20" s="150" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D20" s="151" t="n"/>
+      <c r="E20" s="150" t="inlineStr">
+        <is>
+          <t>22002</t>
+        </is>
+      </c>
+      <c r="F20" s="150" t="inlineStr"/>
+      <c r="G20" s="150" t="inlineStr"/>
+      <c r="H20" s="151" t="n"/>
+      <c r="I20" s="151" t="n"/>
+      <c r="J20" s="150" t="inlineStr">
+        <is>
+          <t>INSERT</t>
+        </is>
+      </c>
+      <c r="K20" s="150" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="L20" s="150" t="inlineStr">
+        <is>
+          <t>Sea</t>
+        </is>
+      </c>
+      <c r="M20" s="152" t="n">
+        <v>45554</v>
+      </c>
+      <c r="N20" s="150" t="n"/>
+      <c r="O20" s="150" t="n"/>
+      <c r="P20" s="151" t="n"/>
+      <c r="Q20" s="150" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="R20" s="151" t="n"/>
+      <c r="S20" s="153" t="n">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1">
+      <c r="B21" s="154" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C21" s="155" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="156" t="n"/>
+      <c r="E21" s="155" t="inlineStr">
+        <is>
+          <t>22002</t>
+        </is>
+      </c>
+      <c r="F21" s="155" t="inlineStr"/>
+      <c r="G21" s="155" t="inlineStr"/>
+      <c r="H21" s="156" t="n"/>
+      <c r="I21" s="156" t="n"/>
+      <c r="J21" s="155" t="inlineStr">
+        <is>
+          <t>INSERT</t>
+        </is>
+      </c>
+      <c r="K21" s="155" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="L21" s="155" t="inlineStr">
+        <is>
+          <t>Sea</t>
+        </is>
+      </c>
+      <c r="M21" s="157" t="n">
+        <v>45554</v>
+      </c>
+      <c r="N21" s="155" t="n"/>
+      <c r="O21" s="155" t="n"/>
+      <c r="P21" s="156" t="n"/>
+      <c r="Q21" s="155" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="R21" s="156" t="n"/>
+      <c r="S21" s="158" t="n">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="22" ht="14" customHeight="1">
+      <c r="B22" s="13" t="n"/>
+      <c r="C22" s="14" t="n"/>
+      <c r="D22" s="9" t="n"/>
+      <c r="E22" s="15" t="n"/>
+      <c r="F22" s="15" t="n"/>
+      <c r="G22" s="8" t="n"/>
+      <c r="H22" s="8" t="n"/>
+      <c r="I22" s="8" t="n"/>
+      <c r="J22" s="10" t="n"/>
+      <c r="K22" s="101" t="n"/>
+      <c r="L22" s="9" t="n"/>
+      <c r="M22" s="159" t="n"/>
+      <c r="N22" s="159" t="n"/>
+      <c r="O22" s="31" t="n"/>
+      <c r="P22" s="160" t="n"/>
+      <c r="Q22" s="160" t="n"/>
+      <c r="R22" s="160" t="n"/>
+      <c r="S22" s="161" t="n"/>
+    </row>
+    <row r="23" ht="14" customFormat="1" customHeight="1" s="2" thickBot="1">
+      <c r="B23" s="13" t="n"/>
+      <c r="C23" s="14" t="n"/>
+      <c r="D23" s="9" t="n"/>
+      <c r="E23" s="15" t="n"/>
+      <c r="F23" s="15" t="n"/>
+      <c r="G23" s="8" t="n"/>
+      <c r="H23" s="8" t="n"/>
+      <c r="I23" s="8" t="n"/>
+      <c r="J23" s="10" t="n"/>
+      <c r="K23" s="101" t="n"/>
+      <c r="L23" s="9" t="n"/>
+      <c r="M23" s="159" t="n"/>
+      <c r="N23" s="159" t="n"/>
+      <c r="O23" s="31" t="n"/>
+      <c r="P23" s="160" t="n"/>
+      <c r="Q23" s="160" t="n"/>
+      <c r="R23" s="160" t="n"/>
+      <c r="S23" s="161" t="n"/>
+    </row>
+    <row r="24" ht="16" customFormat="1" customHeight="1" s="2">
+      <c r="M24" s="17" t="n"/>
+      <c r="N24" s="33" t="n"/>
+      <c r="O24" s="33" t="n"/>
+      <c r="P24" s="79" t="inlineStr">
         <is>
           <t>合计</t>
         </is>
       </c>
-      <c r="Q20" s="36" t="inlineStr">
+      <c r="Q24" s="36" t="inlineStr">
         <is>
           <t>( TOTAL)</t>
         </is>
       </c>
-      <c r="R20" s="157" t="n">
-        <v>20000</v>
-      </c>
-      <c r="S20" s="117" t="n"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="85" t="inlineStr">
+      <c r="R24" s="162" t="n">
+        <v>66300</v>
+      </c>
+      <c r="S24" s="117" t="n"/>
+    </row>
+    <row r="25" ht="14" customHeight="1">
+      <c r="B25" s="85" t="inlineStr">
         <is>
           <t>说明（NOTE）:</t>
         </is>
       </c>
-      <c r="C21" s="86" t="n"/>
-      <c r="D21" s="86" t="n"/>
-      <c r="E21" s="86" t="n"/>
-      <c r="F21" s="87" t="n"/>
-      <c r="G21" s="87" t="n"/>
-      <c r="H21" s="87" t="n"/>
-      <c r="I21" s="87" t="n"/>
-      <c r="J21" s="88" t="n"/>
-      <c r="K21" s="102" t="n"/>
-      <c r="L21" s="89" t="n"/>
-      <c r="M21" s="90" t="n"/>
-      <c r="N21" s="33" t="n"/>
-      <c r="O21" s="33" t="n"/>
-      <c r="P21" s="158" t="n"/>
-      <c r="Q21" s="43" t="n"/>
-      <c r="R21" s="43" t="n"/>
-      <c r="S21" s="44" t="n"/>
-    </row>
-    <row r="22" ht="14" customHeight="1">
-      <c r="B22" s="110" t="n"/>
-      <c r="C22" s="111" t="n"/>
-      <c r="D22" s="111" t="n"/>
-      <c r="E22" s="111" t="n"/>
-      <c r="F22" s="111" t="n"/>
-      <c r="G22" s="111" t="n"/>
-      <c r="H22" s="111" t="n"/>
-      <c r="I22" s="111" t="n"/>
-      <c r="J22" s="111" t="n"/>
-      <c r="K22" s="111" t="n"/>
-      <c r="L22" s="111" t="n"/>
-      <c r="M22" s="112" t="n"/>
-    </row>
-    <row r="23" ht="14" customFormat="1" customHeight="1" s="2" thickBot="1">
-      <c r="B23" s="110" t="n"/>
-      <c r="C23" s="111" t="n"/>
-      <c r="D23" s="111" t="n"/>
-      <c r="E23" s="111" t="n"/>
-      <c r="F23" s="111" t="n"/>
-      <c r="G23" s="111" t="n"/>
-      <c r="H23" s="111" t="n"/>
-      <c r="I23" s="111" t="n"/>
-      <c r="J23" s="111" t="n"/>
-      <c r="K23" s="111" t="n"/>
-      <c r="L23" s="111" t="n"/>
-      <c r="M23" s="112" t="n"/>
-      <c r="P23" s="83" t="inlineStr">
+      <c r="C25" s="86" t="n"/>
+      <c r="D25" s="86" t="n"/>
+      <c r="E25" s="86" t="n"/>
+      <c r="F25" s="87" t="n"/>
+      <c r="G25" s="87" t="n"/>
+      <c r="H25" s="87" t="n"/>
+      <c r="I25" s="87" t="n"/>
+      <c r="J25" s="88" t="n"/>
+      <c r="K25" s="102" t="n"/>
+      <c r="L25" s="89" t="n"/>
+      <c r="M25" s="90" t="n"/>
+      <c r="N25" s="33" t="n"/>
+      <c r="O25" s="33" t="n"/>
+      <c r="P25" s="163" t="n"/>
+      <c r="Q25" s="43" t="n"/>
+      <c r="R25" s="43" t="n"/>
+      <c r="S25" s="44" t="n"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="110" t="n"/>
+      <c r="C26" s="111" t="n"/>
+      <c r="D26" s="111" t="n"/>
+      <c r="E26" s="111" t="n"/>
+      <c r="F26" s="111" t="n"/>
+      <c r="G26" s="111" t="n"/>
+      <c r="H26" s="111" t="n"/>
+      <c r="I26" s="111" t="n"/>
+      <c r="J26" s="111" t="n"/>
+      <c r="K26" s="111" t="n"/>
+      <c r="L26" s="111" t="n"/>
+      <c r="M26" s="112" t="n"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="110" t="n"/>
+      <c r="C27" s="111" t="n"/>
+      <c r="D27" s="111" t="n"/>
+      <c r="E27" s="111" t="n"/>
+      <c r="F27" s="111" t="n"/>
+      <c r="G27" s="111" t="n"/>
+      <c r="H27" s="111" t="n"/>
+      <c r="I27" s="111" t="n"/>
+      <c r="J27" s="111" t="n"/>
+      <c r="K27" s="111" t="n"/>
+      <c r="L27" s="111" t="n"/>
+      <c r="M27" s="112" t="n"/>
+      <c r="P27" s="83" t="inlineStr">
         <is>
           <t>订单签发人 (BY):</t>
         </is>
       </c>
-      <c r="Q23" s="159" t="n"/>
-      <c r="R23" s="160" t="inlineStr">
+      <c r="Q27" s="164" t="n"/>
+      <c r="R27" s="165" t="inlineStr">
         <is>
           <t>Tim Qi</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="16" customFormat="1" customHeight="1" s="2">
-      <c r="B24" s="113" t="n"/>
-      <c r="C24" s="114" t="n"/>
-      <c r="D24" s="114" t="n"/>
-      <c r="E24" s="114" t="n"/>
-      <c r="F24" s="114" t="n"/>
-      <c r="G24" s="114" t="n"/>
-      <c r="H24" s="114" t="n"/>
-      <c r="I24" s="114" t="n"/>
-      <c r="J24" s="114" t="n"/>
-      <c r="K24" s="114" t="n"/>
-      <c r="L24" s="114" t="n"/>
-      <c r="M24" s="115" t="n"/>
-      <c r="N24" s="19" t="n"/>
-      <c r="O24" s="19" t="n"/>
-      <c r="Q24" s="161" t="n"/>
-      <c r="R24" s="162" t="n"/>
-      <c r="S24" s="163" t="n"/>
-    </row>
-    <row r="25" ht="14" customHeight="1">
-      <c r="B25" s="4" t="n"/>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="4" t="n"/>
-      <c r="E25" s="4" t="n"/>
-      <c r="F25" s="24" t="n"/>
-      <c r="G25" s="24" t="n"/>
-      <c r="H25" s="24" t="n"/>
-      <c r="I25" s="24" t="n"/>
-      <c r="J25" s="4" t="n"/>
-      <c r="K25" s="103" t="n"/>
-      <c r="L25" s="18" t="n"/>
-      <c r="M25" s="18" t="n"/>
-      <c r="N25" s="18" t="n"/>
-      <c r="O25" s="18" t="n"/>
-      <c r="P25" s="4" t="n"/>
-      <c r="Q25" s="164" t="n"/>
-      <c r="R25" s="164" t="n"/>
-      <c r="S25" s="165" t="n"/>
-    </row>
-    <row r="26">
-      <c r="B26" s="19" t="inlineStr">
+    <row r="28">
+      <c r="B28" s="113" t="n"/>
+      <c r="C28" s="114" t="n"/>
+      <c r="D28" s="114" t="n"/>
+      <c r="E28" s="114" t="n"/>
+      <c r="F28" s="114" t="n"/>
+      <c r="G28" s="114" t="n"/>
+      <c r="H28" s="114" t="n"/>
+      <c r="I28" s="114" t="n"/>
+      <c r="J28" s="114" t="n"/>
+      <c r="K28" s="114" t="n"/>
+      <c r="L28" s="114" t="n"/>
+      <c r="M28" s="115" t="n"/>
+      <c r="N28" s="19" t="n"/>
+      <c r="O28" s="19" t="n"/>
+      <c r="Q28" s="166" t="n"/>
+      <c r="R28" s="167" t="n"/>
+      <c r="S28" s="168" t="n"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="4" t="n"/>
+      <c r="C29" s="4" t="n"/>
+      <c r="D29" s="4" t="n"/>
+      <c r="E29" s="4" t="n"/>
+      <c r="F29" s="24" t="n"/>
+      <c r="G29" s="24" t="n"/>
+      <c r="H29" s="24" t="n"/>
+      <c r="I29" s="24" t="n"/>
+      <c r="J29" s="4" t="n"/>
+      <c r="K29" s="103" t="n"/>
+      <c r="L29" s="18" t="n"/>
+      <c r="M29" s="18" t="n"/>
+      <c r="N29" s="18" t="n"/>
+      <c r="O29" s="18" t="n"/>
+      <c r="P29" s="4" t="n"/>
+      <c r="Q29" s="169" t="n"/>
+      <c r="R29" s="169" t="n"/>
+      <c r="S29" s="170" t="n"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">    Please notify us immediately if you are unable to deliver as specified.</t>
         </is>
       </c>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="n"/>
-      <c r="E26" s="4" t="n"/>
-      <c r="F26" s="24" t="n"/>
-      <c r="G26" s="24" t="n"/>
-      <c r="H26" s="24" t="n"/>
-      <c r="I26" s="24" t="n"/>
-      <c r="J26" s="4" t="n"/>
-      <c r="K26" s="104" t="n"/>
-      <c r="L26" s="4" t="n"/>
-      <c r="P26" s="166" t="inlineStr">
+      <c r="C30" s="4" t="n"/>
+      <c r="D30" s="4" t="n"/>
+      <c r="E30" s="4" t="n"/>
+      <c r="F30" s="24" t="n"/>
+      <c r="G30" s="24" t="n"/>
+      <c r="H30" s="24" t="n"/>
+      <c r="I30" s="24" t="n"/>
+      <c r="J30" s="4" t="n"/>
+      <c r="K30" s="104" t="n"/>
+      <c r="L30" s="4" t="n"/>
+      <c r="P30" s="171" t="inlineStr">
         <is>
           <t>订货日期 (ORDER DATE):</t>
         </is>
       </c>
-      <c r="Q26" s="160" t="n"/>
-      <c r="R26" s="167" t="n">
+      <c r="Q30" s="165" t="n"/>
+      <c r="R30" s="172" t="n">
         <v>45553</v>
       </c>
-      <c r="S26" s="167" t="n"/>
+      <c r="S30" s="172" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>